<commit_message>
I know the structure of the file rCGH needs as input. maybe I can use my data to create it.
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/review_packages_R.xlsx
+++ b/docs/docs_I_made/review_packages_R.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>output</t>
-  </si>
-  <si>
-    <t>résolution</t>
   </si>
   <si>
     <t>arm-level</t>
@@ -58,15 +55,6 @@
   <si>
     <t>perform relative or absolute copy-number analysis
 three copy-number modelization methods</t>
-  </si>
-  <si>
-    <t>plateforme</t>
-  </si>
-  <si>
-    <t>marche sur windows</t>
-  </si>
-  <si>
-    <t>ne marche pas sur windows</t>
   </si>
   <si>
     <t xml:space="preserve">a JSON in command line , an object on R:
@@ -97,6 +85,27 @@
   <si>
     <t xml:space="preserve">Affymetrix SNP6.0 and cytoScanHD probeset.txt, cychp.txt, and cnchp.txt files exported from ChAS or Affymetrix Power Tools.
  rCGH also supports custom arrays, provided data complies with the expected format. </t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>works on windows</t>
+  </si>
+  <si>
+    <t>doesn't work on windows</t>
+  </si>
+  <si>
+    <t>analyzing and interactively visualizing genomic profiles
+ generated through aCGH arrays.
+All the steps required for individual genomic profiles analysis:
+reading files , 
+profiles segmentation, 
+gene annotations
+Also, it provides some visualization functions for individual profile inerpretation</t>
   </si>
 </sst>
 </file>
@@ -420,7 +429,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,10 +451,10 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="315" x14ac:dyDescent="0.25">
@@ -453,16 +462,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -470,24 +479,27 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>